<commit_message>
added attribute disabled for button in worker component
</commit_message>
<xml_diff>
--- a/app/public/file/file.xlsx
+++ b/app/public/file/file.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4057" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4057" uniqueCount="499">
   <si>
     <t>PROCES</t>
   </si>
@@ -1525,6 +1525,15 @@
   </si>
   <si>
     <t>IZABELA DĄBROWSKA</t>
+  </si>
+  <si>
+    <t>Dorota bardzo dobrze wykonuje swoje obowiązki. Stara się być pomocna podczas pracy w swoim zespole. Swoją pracę wykonuje bardzo starannie</t>
+  </si>
+  <si>
+    <t>Zespół jest bardzo zadowolony z pracy Doroty i jej stosunku do obowiązków</t>
+  </si>
+  <si>
+    <t>Sprzątaczka</t>
   </si>
 </sst>
 </file>
@@ -1701,7 +1710,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1801,6 +1810,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2109,8 +2124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U368"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A337" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C372" sqref="C372"/>
+    <sheetView tabSelected="1" topLeftCell="O340" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D336" sqref="D336"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25517,69 +25532,69 @@
         <v>22</v>
       </c>
     </row>
-    <row r="361" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A361" s="19" t="s">
+    <row r="361" spans="1:21" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A361" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B361" s="20" t="s">
+      <c r="B361" s="21" t="s">
         <v>484</v>
       </c>
-      <c r="C361" s="33" t="s">
+      <c r="C361" s="34" t="s">
         <v>485</v>
       </c>
-      <c r="D361" s="32" t="s">
+      <c r="D361" s="34" t="s">
         <v>486</v>
       </c>
-      <c r="E361" s="25">
+      <c r="E361" s="18">
         <v>5879.4590399999997</v>
       </c>
-      <c r="F361" s="25">
+      <c r="F361" s="18">
         <v>34.996780000000001</v>
       </c>
-      <c r="G361" s="27">
-        <v>0</v>
-      </c>
-      <c r="H361" s="27">
-        <v>0</v>
-      </c>
-      <c r="I361" s="27">
-        <v>0</v>
-      </c>
-      <c r="J361" s="27">
-        <v>0</v>
-      </c>
-      <c r="K361" s="27">
-        <v>0</v>
-      </c>
-      <c r="L361" s="27">
-        <v>0</v>
-      </c>
-      <c r="M361" s="27">
-        <v>0</v>
-      </c>
-      <c r="N361" s="27">
-        <v>0</v>
-      </c>
-      <c r="O361" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="P361" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q361" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="R361" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="S361" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="T361" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="U361" s="12" t="s">
-        <v>22</v>
+      <c r="G361" s="28">
+        <v>6048</v>
+      </c>
+      <c r="H361" s="28">
+        <v>36</v>
+      </c>
+      <c r="I361" s="28">
+        <v>5484</v>
+      </c>
+      <c r="J361" s="28">
+        <v>33</v>
+      </c>
+      <c r="K361" s="28">
+        <v>5484</v>
+      </c>
+      <c r="L361" s="28">
+        <v>33</v>
+      </c>
+      <c r="M361" s="28">
+        <v>5484</v>
+      </c>
+      <c r="N361" s="28">
+        <v>33</v>
+      </c>
+      <c r="O361" s="16" t="s">
+        <v>450</v>
+      </c>
+      <c r="P361" s="13" t="s">
+        <v>496</v>
+      </c>
+      <c r="Q361" s="35" t="s">
+        <v>476</v>
+      </c>
+      <c r="R361" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="S361" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="T361" s="35" t="s">
+        <v>498</v>
+      </c>
+      <c r="U361" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="362" spans="1:21" x14ac:dyDescent="0.25">
@@ -26051,8 +26066,9 @@
     <hyperlink ref="O248" r:id="rId5"/>
     <hyperlink ref="O31" r:id="rId6"/>
     <hyperlink ref="O221" r:id="rId7"/>
+    <hyperlink ref="O361" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>